<commit_message>
Used Vue.cli created routes
</commit_message>
<xml_diff>
--- a/algorithm/sbfl_template.xlsx
+++ b/algorithm/sbfl_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Shelton\Desktop\BFL-web\algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1681ABE6-3055-47DC-A04D-0EE7748E2EB4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1075E4B2-10AE-4C66-B188-8914ECF833C2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" xr2:uid="{E59993D7-295B-4652-B9DF-ADF51697C417}"/>
   </bookViews>
@@ -30,22 +30,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Something</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>something</t>
+    <t>Email</t>
   </si>
   <si>
-    <t>something bold</t>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>bill@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,6 +63,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -79,14 +93,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,13 +416,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A525C36A-6A05-46C1-9DF1-EB4D9E142951}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -418,7 +439,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>50000</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A381882A-B65D-43C1-9AF1-477CB02B24A0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>